<commit_message>
Minor fixes to burndown chart
</commit_message>
<xml_diff>
--- a/Documentation/Burdown chart.xlsx
+++ b/Documentation/Burdown chart.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Overview" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Hoja 2" sheetId="2" r:id="rId4"/>
+    <sheet state="visible" name="Details" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -65,9 +65,18 @@
     <t>Actualizar Documentos</t>
   </si>
   <si>
+    <t>Actualizar documento Vision</t>
+  </si>
+  <si>
+    <t>Actualizar Documento UC</t>
+  </si>
+  <si>
     <t>P</t>
   </si>
   <si>
+    <t>Actualiazar Documento SAD</t>
+  </si>
+  <si>
     <t>Prioridad 0</t>
   </si>
   <si>
@@ -92,7 +101,10 @@
     <t>Recuperatorios + problemas de setupeo</t>
   </si>
   <si>
-    <t>\+ 0,25</t>
+    <t>\+ 0,25%</t>
+  </si>
+  <si>
+    <t>\+ 0.4%</t>
   </si>
   <si>
     <t>Comparation Calculator</t>
@@ -107,13 +119,19 @@
     <t>Previous Sprint # finished</t>
   </si>
   <si>
-    <t>26/11 - 28/11</t>
+    <t>25/11 - 28/11</t>
   </si>
   <si>
     <t>Present Sprint # finished</t>
   </si>
   <si>
+    <t>29/11 - 2/12</t>
+  </si>
+  <si>
     <t xml:space="preserve">Comparation: </t>
+  </si>
+  <si>
+    <t>3/12 - 7/12</t>
   </si>
 </sst>
 </file>
@@ -178,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -197,7 +215,6 @@
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -246,7 +263,7 @@
               <a:defRPr b="0"/>
             </a:pPr>
             <a:r>
-              <a:t>Sprint y # tasks finished</a:t>
+              <a:t>Sprint vs # tasks finished</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -287,11 +304,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="282364374"/>
-        <c:axId val="992907077"/>
+        <c:axId val="487070174"/>
+        <c:axId val="1671265718"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="282364374"/>
+        <c:axId val="487070174"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -306,10 +323,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="992907077"/>
+        <c:crossAx val="1671265718"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="992907077"/>
+        <c:axId val="1671265718"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -340,7 +357,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="282364374"/>
+        <c:crossAx val="487070174"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -401,208 +418,218 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>24</v>
       </c>
+      <c r="B1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="10">
+      <c r="A2" s="9">
         <v>1.0</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="9">
         <v>4.0</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="10">
         <v>0.0</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>25</v>
+      <c r="D2" s="9" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="10">
+      <c r="A3" s="9">
         <v>2.0</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <v>5.0</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="13"/>
+      <c r="C3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="12"/>
     </row>
     <row r="4">
-      <c r="A4" s="10">
+      <c r="A4" s="9">
         <v>3.0</v>
       </c>
-      <c r="B4" s="10">
-        <v>5.0</v>
-      </c>
-      <c r="C4" s="11">
-        <v>0.0</v>
-      </c>
-      <c r="D4" s="13"/>
+      <c r="B4" s="9">
+        <v>7.0</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="12"/>
     </row>
     <row r="5">
-      <c r="A5" s="10"/>
-      <c r="B5" s="14">
+      <c r="A5" s="9"/>
+      <c r="B5" s="13">
         <v>10.0</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
     </row>
     <row r="6">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
     </row>
     <row r="7">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
     </row>
     <row r="8">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
     </row>
     <row r="9">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
     </row>
     <row r="10">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
     </row>
     <row r="11">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
     </row>
     <row r="12">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
     </row>
     <row r="13">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
     </row>
     <row r="14">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
     </row>
     <row r="15">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
     </row>
     <row r="16">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
     </row>
     <row r="17">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
     </row>
     <row r="18">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
     </row>
     <row r="21">
       <c r="H21" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22">
-      <c r="E22" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>29</v>
+      <c r="E22" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I22" s="7">
-        <v>4.0</v>
+        <v>34</v>
+      </c>
+      <c r="I22" s="6">
+        <v>5.0</v>
       </c>
     </row>
     <row r="23">
-      <c r="E23" s="10">
+      <c r="E23" s="9">
         <v>1.0</v>
       </c>
-      <c r="F23" s="10" t="s">
-        <v>31</v>
+      <c r="F23" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I23" s="7">
-        <v>5.0</v>
+        <v>36</v>
+      </c>
+      <c r="I23" s="6">
+        <v>7.0</v>
       </c>
     </row>
     <row r="24">
-      <c r="E24" s="7">
+      <c r="E24" s="9">
         <v>2.0</v>
       </c>
+      <c r="F24" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="H24" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="I24">
         <f>I23/I22</f>
-        <v>1.25</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="25">
-      <c r="E25" s="7">
+      <c r="E25" s="9">
         <v>3.0</v>
       </c>
+      <c r="F25" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -621,7 +648,7 @@
   <cols>
     <col customWidth="1" min="2" max="2" width="22.14"/>
     <col customWidth="1" min="4" max="4" width="30.29"/>
-    <col customWidth="1" min="6" max="6" width="23.57"/>
+    <col customWidth="1" min="6" max="6" width="25.43"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -688,26 +715,36 @@
       </c>
     </row>
     <row r="7">
-      <c r="F7" s="6"/>
+      <c r="F7" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="F8" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="7" t="s">
-        <v>17</v>
+      <c r="A9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10">
       <c r="D10" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11">
       <c r="D11" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12">
-      <c r="D12" s="8" t="s">
-        <v>20</v>
+      <c r="D12" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>